<commit_message>
Add Bulk upload feature for Division, District & BLock
</commit_message>
<xml_diff>
--- a/src/assets/templates/bulk_upload/09_VTAcademicClassSection_Template.xlsx
+++ b/src/assets/templates/bulk_upload/09_VTAcademicClassSection_Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15449768-5D1B-4329-AA0F-756D85476562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{46E4ADA8-9537-4730-AD0A-55261C165246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34C1AD06-1C52-4481-B8FB-5320A193E9FA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="120">
   <si>
     <t>AcademicYear</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>SectorName</t>
+  </si>
+  <si>
+    <t>DateOfAllocation</t>
+  </si>
+  <si>
+    <t>Varchar(150)</t>
   </si>
 </sst>
 </file>
@@ -472,11 +478,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -491,9 +494,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -833,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,201 +850,195 @@
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="J1" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="J2" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>Dropdowns!$H$3:$H$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>F4:F13</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1058,457 +1052,457 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4" style="4" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.28515625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.140625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.5703125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.85546875" style="4" customWidth="1"/>
-    <col min="16" max="16" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.140625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="25.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.42578125" style="4" customWidth="1"/>
-    <col min="20" max="20" width="26.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.28515625" style="4" customWidth="1"/>
-    <col min="22" max="22" width="52.7109375" style="4" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="4" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="26.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.28515625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="52.7109375" style="3" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="R4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="T4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="V4" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="P5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="T5" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="V5" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="P6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="R6" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="T6" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="V6" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="J7" s="6" t="s">
+      <c r="H7" s="4"/>
+      <c r="J7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="V7" s="6" t="s">
+      <c r="V7" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="8" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="N8" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="R8" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="T8" s="3" t="s">
+      <c r="T8" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="P9" s="6" t="s">
+      <c r="P9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="R9" s="6" t="s">
+      <c r="R9" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="T9" s="6" t="s">
+      <c r="T9" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="10" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="P10" s="6" t="s">
+      <c r="P10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="R10" s="6" t="s">
+      <c r="R10" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="T10" s="6" t="s">
+      <c r="T10" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="11" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="P11" s="6" t="s">
+      <c r="P11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="R11" s="6" t="s">
+      <c r="R11" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="T11" s="6" t="s">
+      <c r="T11" s="5" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="N12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="P12" s="6" t="s">
+      <c r="P12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R12" s="6" t="s">
+      <c r="R12" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="T12" s="6" t="s">
+      <c r="T12" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="13" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="N13" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="P13" s="6" t="s">
+      <c r="P13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="T13" s="6" t="s">
+      <c r="T13" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="14" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="N14" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="15" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="L15" s="6" t="s">
+      <c r="L15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N15" s="6" t="s">
+      <c r="N15" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="P15" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="16" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="L16" s="6" t="s">
+      <c r="L16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="N16" s="6" t="s">
+      <c r="N16" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="P16" s="6" t="s">
+      <c r="P16" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="17" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L17" s="6" t="s">
+      <c r="L17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="P17" s="6" t="s">
+      <c r="P17" s="5" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="18" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L18" s="6" t="s">
+      <c r="L18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="N18" s="3" t="s">
+      <c r="N18" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="19" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L19" s="6" t="s">
+      <c r="L19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N19" s="6" t="s">
+      <c r="N19" s="5" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="20" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L20" s="6" t="s">
+      <c r="L20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N20" s="6" t="s">
+      <c r="N20" s="5" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="21" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L21" s="6" t="s">
+      <c r="L21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="N21" s="6" t="s">
+      <c r="N21" s="5" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="22" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L22" s="6" t="s">
+      <c r="L22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="N22" s="6" t="s">
+      <c r="N22" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="23" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L23" s="6" t="s">
+      <c r="L23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="N23" s="6" t="s">
+      <c r="N23" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="24" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L24" s="6" t="s">
+      <c r="L24" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N24" s="6" t="s">
+      <c r="N24" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="25" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L25" s="6" t="s">
+      <c r="L25" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="N25" s="6" t="s">
+      <c r="N25" s="5" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="26" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L26" s="6" t="s">
+      <c r="L26" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="N26" s="6" t="s">
+      <c r="N26" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="27" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L27" s="6" t="s">
+      <c r="L27" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="28" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L28" s="6" t="s">
+      <c r="L28" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="29" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L29" s="6" t="s">
+      <c r="L29" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L30" s="6" t="s">
+      <c r="L30" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="31" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L31" s="6" t="s">
+      <c r="L31" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="32" spans="12:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L32" s="6" t="s">
+      <c r="L32" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="33" spans="12:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="L33" s="6" t="s">
+      <c r="L33" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="34" spans="12:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="L34" s="6" t="s">
+      <c r="L34" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="12:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="L35" s="6" t="s">
+      <c r="L35" s="5" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>